<commit_message>
faz ikiye geçildi. ekran tasarımları yapıldı.
</commit_message>
<xml_diff>
--- a/ArGeTesvikTool.WebUI/wwwroot/file-template/Dışarıda_Geçirilen_Süre_Bildirimi.xlsx
+++ b/ArGeTesvikTool.WebUI/wwwroot/file-template/Dışarıda_Geçirilen_Süre_Bildirimi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TR996928\Documents\Customer\PwC\Borusan\Lojistik\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TR996928\Documents\Visual Studio 2019\Projects\ArGeTesvik.Tool\ArGeTesvikTool.WebUI\wwwroot\file-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693E4C2D-ED69-4675-A759-7ECF683C9F69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFB4563-A1D4-4DEA-9FDA-E2E2F2D6DA9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,18 +36,17 @@
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="162"/>
-          </rPr>
-          <t xml:space="preserve">Bu alana girdiğiniz 
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t>Bu alana girdiğiniz 
 T.C. Kimlik No / Yabancı Kimlik No 
 sistemde kayıtlı olan bir personele ait olmalıdır aksi takdirde ilgili satırın kaydı Başarısız olucaktır.
 T.C. Kimlik No / Yabancı Kimlik No 'lu
-personel sistemde kayıtlı değilse ilk önce sisteme kaydını yapınız.
-</t>
+personel sistemde kayıtlı değilse ilk önce sisteme kaydını yapınız.</t>
         </r>
       </text>
     </comment>
@@ -106,11 +105,10 @@
             <family val="2"/>
             <charset val="162"/>
           </rPr>
-          <t xml:space="preserve">ise ilgili satır için İlişkili Proje Kodu girmenize gerek yoktur.
+          <t>ise ilgili satır için İlişkili Proje Kodu girmenize gerek yoktur.
 Diğer Faaliyet Türleri için
 Bu alana girdiğiniz 
-İlişkili Proje Kodu sistemde kayıtlı olan bir projeye ait olmalıdır aksi takdirde ilgili satırın kaydı başarısız olucaktır
-</t>
+İlişkili Proje Kodu sistemde kayıtlı olan bir projeye ait olmalıdır aksi takdirde ilgili satırın kaydı başarısız olucaktır.</t>
         </r>
       </text>
     </comment>
@@ -119,7 +117,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -129,7 +127,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -141,7 +139,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -151,7 +149,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -163,7 +161,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -173,7 +171,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -184,7 +182,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="14"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -194,7 +192,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -206,7 +204,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -216,7 +214,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -227,7 +225,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="14"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -237,7 +235,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -249,7 +247,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -259,7 +257,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -270,7 +268,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="14"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -280,7 +278,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -292,7 +290,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -302,7 +300,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -313,7 +311,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="14"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -323,7 +321,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -335,7 +333,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -345,7 +343,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -356,7 +354,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="14"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -366,7 +364,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -378,7 +376,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -388,7 +386,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -399,7 +397,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="14"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -409,7 +407,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -421,7 +419,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -431,7 +429,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -442,7 +440,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="14"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -452,7 +450,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -464,7 +462,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -474,7 +472,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -485,29 +483,18 @@
         <r>
           <rPr>
             <b/>
-            <sz val="14"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="162"/>
           </rPr>
           <t xml:space="preserve">8
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="162"/>
-          </rPr>
-          <t xml:space="preserve">* Bilimsel İçerikli Etkinlik </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
+* Bilimsel İçerikli Etkinlik </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -518,41 +505,40 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="162"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="14"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="162"/>
-          </rPr>
-          <t xml:space="preserve">9
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="162"/>
-          </rPr>
-          <t xml:space="preserve">*COVID-19 için 10
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t xml:space="preserve"> 9
+* COVID-19 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t>için</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t xml:space="preserve"> 10
 *7263 sayılı Kanun ile getirilen Dışarıda Geçirilen Süre Hakkı </t>
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -563,7 +549,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -574,7 +560,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -585,7 +571,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -596,7 +582,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -609,7 +595,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -623,7 +609,7 @@
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -631,7 +617,7 @@
           </rPr>
           <t>Bu alan için sadece sayısal veri giriniz.
 Örn: 2017
-bu alanın girilmesi zorunludur aksi takdirde ilgili satırın kaydı başarısız olur.</t>
+Bu alanın girilmesi zorunludur aksi takdirde ilgili satırın kaydı başarısız olur.</t>
         </r>
       </text>
     </comment>
@@ -639,23 +625,45 @@
       <text>
         <r>
           <rPr>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="162"/>
-          </rPr>
-          <t xml:space="preserve">Lütfen sadece sayısal olarak değer giriniz. 
-Örnek : Kasım yerine 11 giriniz. </t>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t xml:space="preserve">Bu alan için sadece sayısal veri giriniz.
+Örn: Kasım yerine </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t>11</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t xml:space="preserve"> giriniz.    </t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">   
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
       </text>
@@ -664,7 +672,7 @@
       <text>
         <r>
           <rPr>
-            <sz val="11"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -676,7 +684,7 @@
         <r>
           <rPr>
             <b/>
-            <sz val="11"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -687,7 +695,7 @@
         </r>
         <r>
           <rPr>
-            <sz val="11"/>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -698,17 +706,17 @@
         <r>
           <rPr>
             <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="162"/>
-          </rPr>
-          <t>8,5</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="162"/>
+          </rPr>
+          <t>8.5</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
@@ -759,7 +767,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -767,13 +775,6 @@
       <family val="2"/>
       <charset val="162"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="162"/>
     </font>
     <font>
       <b/>
@@ -784,21 +785,7 @@
       <charset val="162"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="162"/>
-    </font>
-    <font>
       <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
@@ -814,14 +801,6 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="162"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
@@ -901,17 +880,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1192,9 +1172,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1234,7 +1216,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -1242,7 +1224,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -1250,7 +1232,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
@@ -1258,7 +1240,7 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -1266,7 +1248,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -1274,7 +1256,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -1282,7 +1264,7 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
@@ -1290,7 +1272,7 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
@@ -1298,7 +1280,7 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -1306,7 +1288,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
@@ -1314,7 +1296,7 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="4"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
@@ -1322,7 +1304,7 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="4"/>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
@@ -1330,7 +1312,7 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="4"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
@@ -1338,7 +1320,7 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
@@ -1346,7 +1328,7 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="4"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
@@ -1354,7 +1336,7 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="4"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
@@ -1362,7 +1344,7 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
@@ -1370,9 +1352,684 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="6"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="6"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="6"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="6"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="6"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="6"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="6"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="6"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="6"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="6"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="6"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="6"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="6"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="6"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="6"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="6"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="6"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="6"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="6"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="6"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="6"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="6"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="6"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="6"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="6"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="6"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="6"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="6"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="4"/>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="6"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="5"/>
+      <c r="F81" s="6"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="4"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="6"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="4"/>
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="5"/>
+      <c r="F83" s="6"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="4"/>
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="6"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="4"/>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="5"/>
+      <c r="F85" s="6"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="4"/>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="6"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="6"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="4"/>
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="6"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="4"/>
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="6"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="4"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="6"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="6"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="4"/>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="6"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="6"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="4"/>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="4"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="6"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="4"/>
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="6"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="4"/>
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="4"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="6"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="6"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="6"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="4"/>
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="4"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="6"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="6"/>
     </row>
   </sheetData>
+  <dataConsolidate/>
+  <dataValidations count="7">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Hata" error="Bu alan 1 ile 12 arasında sayı değeri kabul etmektedir." sqref="C1" xr:uid="{D73C305C-DDC7-4E72-83E4-9E56D1796F81}">
+      <formula1>1</formula1>
+      <formula2>12</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Hata" error="1-12 arasında bir değer giriniz." promptTitle="Bilgi" prompt="Bu alana sadece sayılar veri giriniz._x000a__x000a_Örn: Kasım yerine 11 giriniz." sqref="E2:E100" xr:uid="{DC5C52D9-1C80-4A54-9770-27CDA286AD6A}">
+      <formula1>1</formula1>
+      <formula2>12</formula2>
+    </dataValidation>
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" errorTitle="Hata" error="Kimlik numarasını kontrol ediniz." promptTitle="Bilgi" prompt="Bu alana girdiğiniz_x000a__x000a_T.C Kimlik No/Yabancı Kimlik No sistemde kayıtlı olan bir personele ait olmalıdır. Aksi taktirde ilgili satırın kaydı başarısız olacaktır._x000a__x000a_T.C Kimlik No/Yabancı Kimlik No'lu personel sistemde kayıtlı değilse sisteme kaydınız yapınız." sqref="A2:A100" xr:uid="{911E2906-18E0-4AFE-9384-F5698FAADE77}">
+      <formula1>10000000000</formula1>
+      <formula2>99999999999</formula2>
+    </dataValidation>
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" errorTitle="Hata" error="Yılı kontrol ediniz." promptTitle="Bilgi" prompt="Bu alanın girilmesi zorunludur. Aksi taktirde ilgili satırın kaydı başarısız olur._x000a__x000a_Bu alan için sadece sayılar veri giriniz._x000a__x000a_Örn: 2017" sqref="D2:D100" xr:uid="{FFDBC13A-7684-4531-9549-5E38D1FBE5D5}">
+      <formula1>1900</formula1>
+      <formula2>2999</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="Faaliyet türü için girilen veri_x000a_* Yüksek lisans eğitimi için 1_x000a_* Doktora eğitimi için 2 _x000a_ise ilgili satır için ilişkin proje kodu girmenize gerek yoktur._x000a__x000a_Bu alana girdiğiniz ilişkili proje kodu sistemde kayıtlı olan bir projeye ait olmalıdır." sqref="B2:B100" xr:uid="{685FB2FE-6928-461F-9461-6754FF1AE44B}"/>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Hata" error="1-12 arasında bir değer giriniz." promptTitle="Bilgi" prompt="Faaliyet türü için girebileceğiniz değerler;_x000a_*Yüksek lisans: 1_x000a_*Doktora: 2_x000a_*Laboratuvar: 3_x000a_*Analiz: 4_x000a_*Test ve Deney: 5_x000a__x000a_Daha fazlası için açıklamaya bakınız." sqref="C2:C100" xr:uid="{2C5F7F99-A7C4-4D60-BB5B-864575888B33}">
+      <formula1>1</formula1>
+      <formula2>12</formula2>
+    </dataValidation>
+    <dataValidation type="custom" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Hata" error="Girdiğiniz değeri kontrol ediniz." promptTitle="Bilgi" prompt="Bu alana sadece sayılar değer giriniz._x000a_Girdiğiniz değerlerin yayına saat yazmayızı._x000a__x000a_Örn: 32  veya 8.5" sqref="F2:F100" xr:uid="{03C6E68E-11D2-4C93-9DEB-56F8640763A2}">
+      <formula1>ISNUMBER(F2)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>